<commit_message>
pb quand plusieurs conditions
</commit_message>
<xml_diff>
--- a/data/questions_combinees.xlsx
+++ b/data/questions_combinees.xlsx
@@ -501,7 +501,7 @@
     <t xml:space="preserve">Quelle structure représentez-vous ?</t>
   </si>
   <si>
-    <t xml:space="preserve">Sélectionner…; Une commune;Une communauté de communes;Une communauté d’agglomération;Une communauté urbaine;Une communauté urbaine;Une métropole;Un syndicat mixte;Un département;Une Région</t>
+    <t xml:space="preserve">Sélectionner…;Une commune;Une communauté de communes;Une communauté d’agglomération;Une communauté urbaine;Une métropole;Un syndicat mixte;Un département;Une Région</t>
   </si>
   <si>
     <t xml:space="preserve">3</t>
@@ -514,7 +514,7 @@
 les 3 choix :</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt; 20 000 Habitants ;20 000-50 000 Habitants ;&gt; 50 000 Habitants</t>
+    <t xml:space="preserve">&lt; 20 000 Habitants;20 000-50 000 Habitants;&gt; 50 000 Habitants</t>
   </si>
   <si>
     <t xml:space="preserve">4</t>
@@ -1040,14 +1040,16 @@
   </sheetPr>
   <dimension ref="A1:L164"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K80" activeCellId="0" sqref="K80"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F75" activeCellId="0" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="63.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="46.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="23.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,7 +1083,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -1107,7 +1109,7 @@
       <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2277,7 +2279,7 @@
       <c r="H80" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K80" s="0" t="s">
+      <c r="K80" s="1" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajout progression thèmes et dots
</commit_message>
<xml_diff>
--- a/data/questions_combinees.xlsx
+++ b/data/questions_combinees.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="307">
   <si>
     <t xml:space="preserve">Numero</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve">Condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remplace</t>
   </si>
   <si>
     <t xml:space="preserve">Theme</t>
@@ -1083,18 +1086,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M164"/>
+  <dimension ref="A1:N164"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H80" activeCellId="0" sqref="H80"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="63.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="46.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="23.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="37.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="63.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="46.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="23.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,83 +1141,83 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="1" t="s">
-        <v>14</v>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="1" t="s">
-        <v>14</v>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>29</v>
@@ -1221,120 +1225,120 @@
       <c r="G6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="1" t="s">
-        <v>14</v>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="1" t="s">
-        <v>14</v>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="1" t="s">
-        <v>14</v>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="1" t="s">
-        <v>14</v>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="H13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="1" t="s">
-        <v>14</v>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>44</v>
@@ -1342,13 +1346,13 @@
       <c r="G15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -1358,249 +1362,252 @@
         <v>49</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>50</v>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>47</v>
+        <v>23</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>48</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="1" t="s">
-        <v>47</v>
+      <c r="E18" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1" t="s">
+      <c r="G19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="1" t="s">
-        <v>47</v>
+      <c r="E20" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="1" t="s">
-        <v>47</v>
+      <c r="E21" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="E22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>59</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="1" t="s">
-        <v>47</v>
+      <c r="E23" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>62</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="H24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="1" t="s">
-        <v>47</v>
+      <c r="E25" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H26" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="H27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="K27" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="1" t="s">
-        <v>68</v>
+      <c r="E28" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="2" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="H31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I31" s="1"/>
       <c r="J31" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="K31" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>82</v>
@@ -1608,578 +1615,578 @@
       <c r="G32" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="H32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I32" s="1"/>
       <c r="J32" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="H33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I33" s="1"/>
       <c r="J33" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="K33" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="I34" s="1"/>
       <c r="J34" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="K34" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1" t="s">
-        <v>78</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I35" s="1"/>
       <c r="J35" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H36" s="1"/>
-      <c r="J36" s="1" t="s">
         <v>94</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I36" s="1"/>
+      <c r="K36" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D37" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="2" t="s">
         <v>98</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L37" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="H37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="1" t="s">
-        <v>96</v>
+      <c r="E38" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="1" t="s">
-        <v>96</v>
+      <c r="E40" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>96</v>
+        <v>28</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="1" t="s">
-        <v>96</v>
+      <c r="E42" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>96</v>
+        <v>28</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>108</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="1" t="s">
-        <v>96</v>
+      <c r="E44" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E45" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="E45" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>111</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="1" t="s">
-        <v>96</v>
+      <c r="E46" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>96</v>
+        <v>28</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>114</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1" t="s">
-        <v>63</v>
+        <v>115</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="1" t="s">
-        <v>96</v>
+      <c r="E48" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>117</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H49" s="1"/>
+        <v>118</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D50" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E50" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>98</v>
+      <c r="F50" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>121</v>
+        <v>99</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D51" s="1" t="s">
-        <v>119</v>
+      <c r="E51" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E52" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>52</v>
+      <c r="F52" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D53" s="1" t="s">
-        <v>119</v>
+      <c r="E53" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F54" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>126</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D55" s="1" t="s">
-        <v>119</v>
+      <c r="E55" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>129</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D57" s="1" t="s">
-        <v>119</v>
+      <c r="E57" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>132</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D59" s="1" t="s">
-        <v>119</v>
+      <c r="E59" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>135</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D61" s="1" t="s">
-        <v>119</v>
+      <c r="E61" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H62" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D63" s="1" t="s">
-        <v>119</v>
+      <c r="E63" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>140</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1" t="s">
-        <v>63</v>
+        <v>141</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D65" s="1" t="s">
-        <v>119</v>
+      <c r="E65" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>143</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H66" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="673.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D67" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E67" s="1" t="s">
@@ -2189,931 +2196,931 @@
         <v>147</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H67" s="1"/>
-      <c r="L67" s="2" t="s">
         <v>148</v>
       </c>
+      <c r="H67" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I67" s="1"/>
+      <c r="M67" s="2" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D68" s="1" t="s">
-        <v>145</v>
+      <c r="E68" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>152</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H69" s="1"/>
+        <v>153</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I69" s="1"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D70" s="1" t="s">
-        <v>145</v>
+      <c r="E70" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H71" s="1"/>
+        <v>156</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I71" s="1"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D72" s="1" t="s">
-        <v>145</v>
+      <c r="E72" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>158</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H73" s="1"/>
+        <v>159</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I73" s="1"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D74" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="K74" s="1" t="s">
-        <v>24</v>
+      <c r="E74" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>145</v>
+        <v>22</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>160</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H75" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I75" s="1"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D76" s="1" t="s">
-        <v>145</v>
+      <c r="E76" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E77" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="E77" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>164</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H77" s="1"/>
+        <v>165</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I77" s="1"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D78" s="1" t="s">
-        <v>145</v>
+      <c r="E78" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>167</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="K79" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I79" s="1" t="s">
         <v>169</v>
+      </c>
+      <c r="L79" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D80" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="E80" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>98</v>
+      <c r="F80" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H80" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L80" s="1" t="s">
-        <v>173</v>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D81" s="1" t="s">
-        <v>171</v>
+      <c r="E81" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>171</v>
+        <v>23</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>101</v>
+        <v>172</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D83" s="1" t="s">
-        <v>171</v>
+      <c r="E83" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>171</v>
+        <v>28</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>178</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H84" s="1"/>
-      <c r="I84" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H84" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D85" s="1" t="s">
-        <v>171</v>
+      <c r="E85" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E86" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="F86" s="1" t="s">
-        <v>111</v>
+      <c r="E86" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>181</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H86" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D87" s="1" t="s">
-        <v>171</v>
+      <c r="E87" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>171</v>
+        <v>28</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>183</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H88" s="1"/>
-      <c r="I88" s="1" t="s">
-        <v>63</v>
+        <v>184</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D89" s="1" t="s">
-        <v>171</v>
+      <c r="E89" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>186</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H90" s="1"/>
+        <v>187</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I90" s="1"/>
     </row>
     <row r="91" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D91" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E91" s="2" t="s">
+      <c r="E91" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>98</v>
+      <c r="F91" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H91" s="1"/>
-      <c r="I91" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H91" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L91" s="1" t="s">
-        <v>190</v>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M91" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D92" s="1" t="s">
-        <v>188</v>
+      <c r="E92" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>188</v>
+        <v>23</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D94" s="1" t="s">
-        <v>188</v>
+      <c r="E94" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="F95" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F95" s="2" t="s">
         <v>195</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H95" s="1"/>
-      <c r="I95" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H95" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D96" s="1" t="s">
-        <v>188</v>
+      <c r="E96" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>188</v>
+        <v>28</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>198</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H97" s="1"/>
-      <c r="I97" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H97" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D98" s="1" t="s">
-        <v>188</v>
+      <c r="E98" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E99" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="F99" s="1" t="s">
-        <v>111</v>
+      <c r="E99" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H99" s="1"/>
-      <c r="I99" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H99" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D100" s="1" t="s">
-        <v>188</v>
+      <c r="E100" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>188</v>
+        <v>28</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>203</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H101" s="1"/>
-      <c r="I101" s="1" t="s">
-        <v>63</v>
+        <v>204</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D102" s="1" t="s">
-        <v>188</v>
+      <c r="E102" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>206</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H103" s="1"/>
+        <v>207</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I103" s="1"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D104" s="1" t="s">
         <v>208</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>209</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>98</v>
+        <v>210</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H104" s="1"/>
-      <c r="I104" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H104" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L104" s="1" t="s">
-        <v>210</v>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M104" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D105" s="1" t="s">
-        <v>208</v>
+      <c r="E105" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>208</v>
+        <v>23</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>209</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>52</v>
+        <v>210</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H106" s="1"/>
-      <c r="I106" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D107" s="1" t="s">
-        <v>208</v>
+      <c r="E107" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>208</v>
+        <v>28</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>215</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H108" s="1"/>
-      <c r="I108" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H108" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D109" s="1" t="s">
-        <v>208</v>
+      <c r="E109" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E110" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="F110" s="1" t="s">
+      <c r="E110" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F110" s="2" t="s">
         <v>218</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H110" s="1"/>
-      <c r="I110" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H110" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I110" s="1"/>
+      <c r="J110" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D111" s="1" t="s">
-        <v>208</v>
+      <c r="E111" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>208</v>
+        <v>28</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H112" s="1"/>
-      <c r="I112" s="1" t="s">
-        <v>63</v>
+        <v>222</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I112" s="1"/>
+      <c r="J112" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D113" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="I113" s="1" t="s">
-        <v>222</v>
+      <c r="E113" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>225</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H114" s="1"/>
+        <v>226</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I114" s="1"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D115" s="1" t="s">
         <v>227</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>228</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>98</v>
+        <v>229</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H115" s="1"/>
-      <c r="I115" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H115" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L115" s="1" t="s">
-        <v>229</v>
+      <c r="I115" s="1"/>
+      <c r="J115" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D116" s="1" t="s">
-        <v>227</v>
+      <c r="E116" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>227</v>
+        <v>23</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>101</v>
+        <v>228</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H117" s="1"/>
-      <c r="I117" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I117" s="1"/>
+      <c r="J117" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D118" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="I118" s="1" t="s">
-        <v>31</v>
+      <c r="E118" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>227</v>
+        <v>28</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>234</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H119" s="1"/>
+        <v>235</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I119" s="1"/>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D120" s="1" t="s">
-        <v>227</v>
+      <c r="E120" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>227</v>
+        <v>28</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>237</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H121" s="1"/>
-      <c r="I121" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H121" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I121" s="1"/>
+      <c r="J121" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D122" s="1" t="s">
-        <v>227</v>
+      <c r="E122" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E123" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F123" s="1" t="s">
-        <v>111</v>
+      <c r="E123" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>240</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H123" s="1"/>
-      <c r="I123" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H123" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I123" s="1"/>
+      <c r="J123" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D124" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="I124" s="1" t="s">
-        <v>31</v>
+      <c r="E124" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J124" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>227</v>
+        <v>28</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>242</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H125" s="1"/>
+        <v>243</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I125" s="1"/>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D126" s="1" t="s">
-        <v>227</v>
+      <c r="E126" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>245</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H127" s="1"/>
+        <v>246</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I127" s="1"/>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D128" s="1" t="s">
         <v>247</v>
       </c>
       <c r="E128" s="1" t="s">
@@ -3123,550 +3130,554 @@
         <v>249</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H128" s="1"/>
-      <c r="L128" s="1" t="s">
         <v>250</v>
       </c>
+      <c r="H128" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I128" s="1"/>
+      <c r="M128" s="1" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D129" s="1" t="s">
-        <v>247</v>
+      <c r="E129" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>248</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H130" s="1"/>
+        <v>253</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I130" s="1"/>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D131" s="1" t="s">
-        <v>247</v>
+      <c r="E131" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>247</v>
+        <v>28</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>256</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H132" s="1"/>
-      <c r="I132" s="1" t="s">
-        <v>18</v>
+        <v>257</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I132" s="1"/>
+      <c r="J132" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D133" s="1" t="s">
-        <v>247</v>
+      <c r="E133" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="F134" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F134" s="2" t="s">
         <v>259</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H134" s="1"/>
-      <c r="I134" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H134" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I134" s="1"/>
+      <c r="J134" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D135" s="1" t="s">
-        <v>247</v>
+      <c r="E135" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="E136" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="F136" s="1" t="s">
-        <v>111</v>
+      <c r="E136" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>262</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H136" s="1"/>
-      <c r="I136" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H136" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I136" s="1"/>
+      <c r="J136" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D137" s="1" t="s">
-        <v>247</v>
+      <c r="E137" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>247</v>
+        <v>28</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>264</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H138" s="1"/>
-      <c r="I138" s="1" t="s">
-        <v>63</v>
+        <v>265</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I138" s="1"/>
+      <c r="J138" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D139" s="1" t="s">
-        <v>247</v>
+      <c r="E139" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="F140" s="1" t="s">
         <v>267</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H140" s="1"/>
+        <v>268</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I140" s="1"/>
     </row>
     <row r="141" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D141" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E141" s="2" t="s">
+      <c r="E141" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="F141" s="1" t="s">
-        <v>98</v>
+      <c r="F141" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H141" s="1"/>
-      <c r="I141" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H141" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L141" s="1" t="s">
-        <v>271</v>
+      <c r="I141" s="1"/>
+      <c r="J141" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M141" s="1" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D142" s="1" t="s">
-        <v>269</v>
+      <c r="E142" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E143" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E143" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="F143" s="1" t="s">
-        <v>52</v>
+      <c r="F143" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H143" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I143" s="1"/>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D144" s="1" t="s">
-        <v>269</v>
+      <c r="E144" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>269</v>
+        <v>28</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>276</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H145" s="1"/>
-      <c r="I145" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="H145" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I145" s="1"/>
+      <c r="J145" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D146" s="1" t="s">
-        <v>269</v>
+      <c r="E146" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E147" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="F147" s="1" t="s">
-        <v>111</v>
+      <c r="E147" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>279</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H147" s="1"/>
-      <c r="I147" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H147" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I147" s="1"/>
+      <c r="J147" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D148" s="1" t="s">
-        <v>269</v>
+      <c r="E148" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>269</v>
+        <v>28</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>281</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H149" s="1"/>
-      <c r="I149" s="1" t="s">
-        <v>63</v>
+        <v>282</v>
+      </c>
+      <c r="H149" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I149" s="1"/>
+      <c r="J149" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D150" s="1" t="s">
-        <v>269</v>
+      <c r="E150" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>284</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H151" s="1"/>
+        <v>285</v>
+      </c>
+      <c r="H151" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I151" s="1"/>
     </row>
     <row r="152" customFormat="false" ht="281.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D152" s="1" t="s">
         <v>286</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>287</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>98</v>
+        <v>288</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H152" s="1"/>
-      <c r="I152" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H152" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L152" s="2" t="s">
-        <v>288</v>
+      <c r="I152" s="1"/>
+      <c r="J152" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M152" s="2" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D153" s="1" t="s">
-        <v>286</v>
+      <c r="E153" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>286</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="D154" s="2"/>
       <c r="E154" s="1" t="s">
         <v>287</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>52</v>
+        <v>288</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H154" s="1"/>
-      <c r="I154" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
+      </c>
+      <c r="H154" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I154" s="1"/>
+      <c r="J154" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D155" s="1" t="s">
-        <v>286</v>
+      <c r="E155" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>286</v>
+        <v>28</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>294</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H156" s="1"/>
-      <c r="I156" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H156" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I156" s="1"/>
+      <c r="J156" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D157" s="1" t="s">
-        <v>286</v>
+      <c r="E157" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>286</v>
+        <v>28</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>297</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H158" s="1"/>
-      <c r="I158" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="H158" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="I158" s="1"/>
+      <c r="J158" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D159" s="1" t="s">
-        <v>286</v>
+      <c r="E159" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="E160" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="F160" s="1" t="s">
-        <v>111</v>
+      <c r="E160" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F160" s="2" t="s">
+        <v>300</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H160" s="1"/>
-      <c r="I160" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H160" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I160" s="1"/>
+      <c r="J160" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D161" s="1" t="s">
-        <v>286</v>
+      <c r="E161" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>286</v>
+        <v>28</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>302</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H162" s="1"/>
+        <v>303</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I162" s="1"/>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D163" s="1" t="s">
-        <v>286</v>
+      <c r="E163" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>286</v>
+        <v>304</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>305</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H164" s="1"/>
+        <v>306</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I164" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
A la recherche de la soluce pour substitution question
</commit_message>
<xml_diff>
--- a/data/questions_combinees.xlsx
+++ b/data/questions_combinees.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="305">
   <si>
     <t xml:space="preserve">Numero</t>
   </si>
@@ -87,7 +87,7 @@
 Concrètement, il s’agit de combiner différentes expertises pour envisager des solutions globales : qualité du cadre de vie, revitalisation de quartier, développement des mobilités douces, Nature en ville, protection de la biodiversité, gestion des nuisances, gestion des déchets du BTP, etc. Cette approche s’applique aussi bien à l’échelle du quartier (écoquartiers) que de l’îlot (cour d’école résiliente). </t>
   </si>
   <si>
-    <t xml:space="preserve">8a</t>
+    <t xml:space="preserve">8.1</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
@@ -102,10 +102,10 @@
     <t xml:space="preserve">o</t>
   </si>
   <si>
-    <t xml:space="preserve">8.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8;q8a</t>
+    <t xml:space="preserve">8.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8;q8.1</t>
   </si>
   <si>
     <t xml:space="preserve">Oui</t>
@@ -123,7 +123,7 @@
     <t xml:space="preserve">Multichoix</t>
   </si>
   <si>
-    <t xml:space="preserve">8.2</t>
+    <t xml:space="preserve">8.3</t>
   </si>
   <si>
     <t xml:space="preserve">Aménagement : Avez-vous réalisé des projets concrets en faveur des thématiques suivantes ?</t>
@@ -187,16 +187,16 @@
 ||S’anticipe par la mise en place d’un cadre structurant, en concertation avec les acteurs concernés. </t>
   </si>
   <si>
-    <t xml:space="preserve">5a</t>
+    <t xml:space="preserve">5.1</t>
   </si>
   <si>
     <t xml:space="preserve">Oui;Non;Je ne sais pas;Non applicable à l’échelle de mon syndicat (SSI syndicat)</t>
   </si>
   <si>
-    <t xml:space="preserve">5b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5;q5a</t>
+    <t xml:space="preserve">5.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5;q5.1</t>
   </si>
   <si>
     <t xml:space="preserve">Transition : Précisez les démarches entreprises à
@@ -330,8 +330,7 @@
     <t xml:space="preserve">Gestion intégrée de l’eau</t>
   </si>
   <si>
-    <t xml:space="preserve">Avez-vous élaboré une stratégie de gestion durable de l’eau et
-des milieux aquatiques sur votre territoire ?</t>
+    <t xml:space="preserve">Avez-vous élaboré une stratégie de gestion durable de l’eau et des milieux aquatiques sur votre territoire ?</t>
   </si>
   <si>
     <t xml:space="preserve">Oui;Non;Je ne sais pas</t>
@@ -340,16 +339,13 @@
     <t xml:space="preserve">L’eau est l’un des principaux marqueurs du changement climatique et de ses conséquences, qu’il s’agisse de manque ou d’excès d’eau. Accroître la résilience des territoires pour l’eau nécessite de développer des stratégies de gestion intégrée des ressources en eau et des milieux aquatiques, de faire évoluer les pratiques en décloisonnant les domaines de l’eau et de l’aménagement, ou encore en mobilisant des solutions d’adaptation fondées sur la nature.</t>
   </si>
   <si>
-    <t xml:space="preserve">33a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non applicable à l’échelle de mon syndicat (SSI syndicat)</t>
-  </si>
-  <si>
     <t xml:space="preserve">33.1</t>
   </si>
   <si>
-    <t xml:space="preserve">33;q33a</t>
+    <t xml:space="preserve">33.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33;q33.1</t>
   </si>
   <si>
     <t xml:space="preserve">Eau : Précisez les démarches entreprises parmi les propositions ci-après</t>
@@ -358,7 +354,7 @@
     <t xml:space="preserve">Nous connaissons les aléas climatiques (sécheresse, pluies intenses, tempêtes, etc.) et leurs conséquences sur la disponibilité de la ressource en eau, sur nos systèmes d’eau et d’assainissement, sur la gestion des eaux pluviales, sur le risque inondation;Un diagnostic de disponibilité de la ressource en eau (état quantitatif des masses d’eaux) et des besoins en eau a été établi;Une stratégie territoriale de gestion de l’eau et/ou un Projet de Territoire pour la Gestion de l'Eau (PTGE) ont été élaborés;Nous avons réalisé un schéma directeur d’alimentation en eau potable et/ou d’assainissement (y.c. inventaires des ouvrages sensibles) et programmé des actions d’adaptation ou de prévention des risque;Nous disposons d’un Schéma Directeur de Gestion des Eaux Pluviales (SDGEP);Nos stratégies de gestion de la ressource en eau et des eaux pluviales s’intègrent dans nos documents de planification;Nous disposons d’un diagnostic territorial identifiant les enjeux liés aux milieux aquatiques et à la prévention des inondations (GEMAPI);Nous avons élaboré une stratégie et plan d’actions en faveur de la préservation/restauration des milieux aquatiques et de la prévention des inondations (GEMAPI);La gouvernance pour l’exercice de la GEMAPI est établie;Nous associons régulièrement les parties prenantes dans les projets</t>
   </si>
   <si>
-    <t xml:space="preserve">33.2</t>
+    <t xml:space="preserve">33.3</t>
   </si>
   <si>
     <t xml:space="preserve">Eau: Quels projets avez-vous d’ores et déjà réalisés ?</t>
@@ -408,13 +404,13 @@
     <t xml:space="preserve">Des aléas d’origine naturelle ou anthropique endommagent les infrastructures bâtimentaires ou de transport. Urbanisation, artificialisation des sols, manque de suivi des ouvrages critiques, sous-estimation de la vulnérabilité de l’environnement et changement climatique aggravent ce phénomène. Le maintien des structures en bon état mobilise des ressources importantes pour les collectivités (financières, matériaux et énergie). Si les solutions d'entretien les moins couteuses sont souvent les plus économes en ressources &amp; énergie et présentent donc le meilleur bilan carbone, sauvegarder le patrimoine passe invariablement par la prise en compte de la résilience dans les investissements (travaux neufs, maintenance ou réhabilitation).</t>
   </si>
   <si>
-    <t xml:space="preserve">24a</t>
-  </si>
-  <si>
     <t xml:space="preserve">24.1</t>
   </si>
   <si>
-    <t xml:space="preserve">24;q24a</t>
+    <t xml:space="preserve">24.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24;q24.1</t>
   </si>
   <si>
     <t xml:space="preserve">Infrastructures :  Prenez-vous en compte le changement climatique dans la gestion du patrimoine existant ? (Parcs bâtimentaires et parcs infrastructures de transport i.e. réseaux routiers et accessoires, ponts, ports et voies
@@ -424,7 +420,7 @@
     <t xml:space="preserve">Le gestionnaire a recensé l’ensemble des constructions;Le gestionnaire a identifié les ouvrages, équipements ou bâtiments sensibles et vulnérables;Le gestionnaire dispose d’une bonne connaissance des aléas climatiques et de leurs impacts sur le parc (exposition et vulnérabilité);Le gestionnaire a programmé des actions de prévention des risques liés au changement climatique (réduction de la vulnérabilité, renforcement ou adaptation des ouvrages, remplacement d’équipements, adaptation de l’exploitation)</t>
   </si>
   <si>
-    <t xml:space="preserve">24.2</t>
+    <t xml:space="preserve">24.3</t>
   </si>
   <si>
     <t xml:space="preserve">Infrastructures : Mettez-vous en œuvre une politique de construction bas carbone pour vos réseaux routiers, ouvrages d’art et parc bâtimentaire ? [Exemples de leviers d’actions : limiter le transport des matériaux, préserver les puits de carbone, compenser les émissions de gaz à effet de serre, utiliser des matériaux recyclés et biosourcés, viser la neutralité carbone via l’isolation, etc.]</t>
@@ -433,7 +429,7 @@
     <t xml:space="preserve">Le gestionnaire intègre ces leviers dès la conception des projets (construction et rénovation);Le gestionnaire intègre ces leviers dans les critères de choix d’entreprises de travaux;Le gestionnaire intègre ces leviers dans les modalités de gestion courante du parc (entretien courant, exploitation);Le gestionnaire s’appuie sur un bilan carbone pour objectiver chaque étape (conception, réalisation des travaux, gestion courante)</t>
   </si>
   <si>
-    <t xml:space="preserve">24.3</t>
+    <t xml:space="preserve">24.4</t>
   </si>
   <si>
     <t xml:space="preserve">Infrastructures :  Prenez-vous en compte le changement climatique dans la gestion du patrimoine existant ? (Parcs bâtimentaires)</t>
@@ -442,7 +438,7 @@
     <t xml:space="preserve">Le gestionnaire a recensé l’ensemble des constructions;Le gestionnaire a identifié les bâtiments sensibles et vulnérables;Le gestionnaire a une bonne connaissance des aléas climatiques et de leurs impacts sur le parc bâti (exposition et vulnérabilité);Le gestionnaire a programmé des actions de prévention des risques liés au changement climatique</t>
   </si>
   <si>
-    <t xml:space="preserve">24.4</t>
+    <t xml:space="preserve">24.5</t>
   </si>
   <si>
     <t xml:space="preserve">Infrastructures : Mettez-vous en œuvre une politique de construction bas carbone ?  (Parcs bâtimentaires)</t>
@@ -562,20 +558,19 @@
     <t xml:space="preserve">Gestion du littoral</t>
   </si>
   <si>
-    <t xml:space="preserve">Avez-vous engagé une démarche de gestion intégrée de la
-zone côtière ? Et/ou de résilience du territoire Gestion du littoral ?</t>
+    <t xml:space="preserve">Avez-vous engagé une démarche de gestion intégrée de la zone côtière ? Et/ou de résilience du territoire Gestion du littoral ?</t>
   </si>
   <si>
     <t xml:space="preserve">Aménager les espaces littoraux relève du défi ; les multiples pressions qui s’y exercent (élévation du niveau de la mer notamment) étant appelées à s’amplifier avec le changement climatique.</t>
   </si>
   <si>
-    <t xml:space="preserve">36a</t>
-  </si>
-  <si>
     <t xml:space="preserve">36.1</t>
   </si>
   <si>
-    <t xml:space="preserve">36;q36a</t>
+    <t xml:space="preserve">36.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36;q36.1</t>
   </si>
   <si>
     <t xml:space="preserve">Gestion du littoral : Précisez les démarches entreprises parmi les propositions ci-après</t>
@@ -615,20 +610,19 @@
     <t xml:space="preserve">Mobilités décarbonées</t>
   </si>
   <si>
-    <t xml:space="preserve">Avez-vous élaboré une stratégie en faveur des mobilités
-décarbonées ?</t>
+    <t xml:space="preserve">Avez-vous élaboré une stratégie en faveur des mobilités décarbonées ?</t>
   </si>
   <si>
     <t xml:space="preserve">L’objectif de neutralité carbone à horizon 2050 implique d’importants changements sur l’organisation des systèmes de transports, les usages et comportements, ainsi que les choix technologiques associés. Tous les leviers (report modal, taux de remplissage, efficacité énergétique, sobriété des déplacements) doivent être mobilisés, à la fois pour les voyageurs et les marchandises.</t>
   </si>
   <si>
-    <t xml:space="preserve">21a</t>
-  </si>
-  <si>
     <t xml:space="preserve">21.1</t>
   </si>
   <si>
-    <t xml:space="preserve">21;q21a</t>
+    <t xml:space="preserve">21.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21;q21.1</t>
   </si>
   <si>
     <t xml:space="preserve">Mobilités :  Précisez les démarches entreprises parmi les
@@ -638,7 +632,7 @@
     <t xml:space="preserve">Nous disposons d’une bonne connaissance des pratiques de déplacements sur notre territoire;Nous avons élaboré une stratégie sur les mobilités décarbonées;Notre stratégie et nos actions sur les mobilités s’articulent avec d’autres politiques publiques territoriales (énergie, aménagement, urbanisme);Nous utilisons le numérique pour développer des services de mobilités;Nous évaluons les projets et politiques en vue de les faire évoluer</t>
   </si>
   <si>
-    <t xml:space="preserve">21.2</t>
+    <t xml:space="preserve">21.3</t>
   </si>
   <si>
     <t xml:space="preserve">Mobilités : Quels projets avez-vous d’ores et déjà réalisés ?</t>
@@ -684,13 +678,13 @@
     <t xml:space="preserve">La crise sanitaire et climatique a accéléré la prise de conscience collective : la nature participe largement à l’équilibre de la vie urbaine et devient un facteur d’attractivité incontournable. Soucieux de la qualité de vie et de la santé de vos concitoyens, vous souhaitez garantir un espace urbain vivable. Vous êtes attachés à la biodiversité, à la résilience de votre territoire, aux solutions douces.</t>
   </si>
   <si>
-    <t xml:space="preserve">30a</t>
-  </si>
-  <si>
     <t xml:space="preserve">30.1</t>
   </si>
   <si>
-    <t xml:space="preserve">30;q30a</t>
+    <t xml:space="preserve">30.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30;q30.1</t>
   </si>
   <si>
     <t xml:space="preserve">Nature :  Précisez les démarches entreprises parmi les propositions ci-après</t>
@@ -742,13 +736,13 @@
     <t xml:space="preserve">Le changement climatique amplifie l’intensité et la fréquence des phénomènes naturels, engendrant des problématiques majeures de sécurité et une augmentation du coût des dommages induits. Les gestionnaires territoriaux sont appelés à réduire la vulnérabilité de leur patrimoine, anticiper et mettre en œuvre des stratégies d’aménagement locales pour s’adapter aux risques naturels.</t>
   </si>
   <si>
-    <t xml:space="preserve">27a</t>
-  </si>
-  <si>
     <t xml:space="preserve">27.1</t>
   </si>
   <si>
-    <t xml:space="preserve">27;q27a</t>
+    <t xml:space="preserve">27.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27;q27.1</t>
   </si>
   <si>
     <t xml:space="preserve">Risques naturels : Précisez les démarches entreprises parmi les propositions ci-après</t>
@@ -757,7 +751,7 @@
     <t xml:space="preserve">Nous disposons d’une bonne connaissance des risques naturels de notre territoire;Nous sommes au fait (via un diagnostic, des études, etc.) des conséquences de ces aléas sur le parc bâtimentaire, les réseaux d’infrastructures de transport, la population;La gestion des risques est intégrée dans nos documents de planification (PLUi et SCOT);Nous avons élaboré une Stratégie Locale de gestion du Risque Inondation (SLGRI);Nous avons élaboré un Programme d'Action pour la Prévention du Risque Inondation (PAPI);Nous exerçons la compétence GEMAPI (systèmes d'endiguement, aménagements hydrauliques, entretiens ou d'aménagements de cours d'eau);Nous avons défini d’un programme d’actions pour la prévention des risques (yc. des inondations, du risque cavité);Nous exerçons la compétence GEMAPI (systèmes d'endiguement, aménagements hydrauliques, entretiens ou d'aménagements de cours d'eau)</t>
   </si>
   <si>
-    <t xml:space="preserve">27.2</t>
+    <t xml:space="preserve">27.3</t>
   </si>
   <si>
     <t xml:space="preserve">Risques naturels : Quels projets avez-vous d’ores et déjà réalisés ?</t>
@@ -807,16 +801,16 @@
     <t xml:space="preserve">En réaffirmant l’objectif de zéro artificialisation nette à l’horizon 2050 et la diminution de moitié du rythme annuel de consommation foncière d’ici 2031, la loi climat et résilience de 2021 appelle les collectivités à repenser en profondeur les modèles d’aménagement du territoire, pour permettre des modes de vie plus sobres et préserver les sols.</t>
   </si>
   <si>
-    <t xml:space="preserve">15a</t>
+    <t xml:space="preserve">15.1</t>
   </si>
   <si>
     <t xml:space="preserve">Oui;Non, notre territoire ne s'inscrit pas encore dans une telle dynamique;Je ne sais pas;Non applicable à l’échelle de mon syndicat (SSI syndicat)</t>
   </si>
   <si>
-    <t xml:space="preserve">15.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15;q15a</t>
+    <t xml:space="preserve">15.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15;q15.1</t>
   </si>
   <si>
     <t xml:space="preserve">Etes-vous engagés dans des démarches destinées à mieux connaître votre foncier ?</t>
@@ -825,7 +819,7 @@
     <t xml:space="preserve">Oui, nous mesurons la consommation foncière en nous appuyant sur des indicateurs;Oui, nous disposons d’un observatoire foncier (pour connaître l’appartenance des terrains, les types d’occupation, les contraintes de constructions, les prix du marché, etc.)</t>
   </si>
   <si>
-    <t xml:space="preserve">15.2</t>
+    <t xml:space="preserve">15.3</t>
   </si>
   <si>
     <t xml:space="preserve">Foncier : Précisez les démarches entreprises parmi les
@@ -874,13 +868,13 @@
     <t xml:space="preserve">Le numérique constitue un levier essentiel pour réussir sa transition écologique. Pour les territoires, l’enjeu ne se limite pas au choix d’innovations technologiques. Il convient de bâtir un projet associant l’ensemble des parties prenantes en intégrant les priorités politiques et les spécifiques locales.</t>
   </si>
   <si>
-    <t xml:space="preserve">12a</t>
-  </si>
-  <si>
     <t xml:space="preserve">12.1</t>
   </si>
   <si>
-    <t xml:space="preserve">12;q12a</t>
+    <t xml:space="preserve">12.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12;q12.1</t>
   </si>
   <si>
     <t xml:space="preserve">Territoire : Précisez les démarches entreprises parmi les propositions ci-après :</t>
@@ -930,17 +924,13 @@
 ||La distribution : favoriser la distribution et la disponibilité des énergies renouvelables et nouveaux carburants. </t>
   </si>
   <si>
-    <t xml:space="preserve">18a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un syndicat mixte
-mixte</t>
-  </si>
-  <si>
     <t xml:space="preserve">18.1</t>
   </si>
   <si>
-    <t xml:space="preserve">18;q18a</t>
+    <t xml:space="preserve">18.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18;q18.1</t>
   </si>
   <si>
     <t xml:space="preserve">Energie : Précisez les démarches entreprises parmi les propositions ci-après</t>
@@ -949,7 +939,7 @@
     <t xml:space="preserve">Nous disposons d’un diagnostic des principaux postes de consommation énergétiques (bâtiment et transports);Nous avons évalué le potentiel de réduction des consommations énergétiques (bâtiments et transports);Nous avons évalué le potentiel de production d’énergie renouvelables à l’échelle du territoire;Nous avons défini un plan d’actions concret en matière de « transition énergétique »;Nous travaillons en concertation avec les parties prenantes internes et externes</t>
   </si>
   <si>
-    <t xml:space="preserve">18.2</t>
+    <t xml:space="preserve">18.3</t>
   </si>
   <si>
     <t xml:space="preserve">Energie : Quels projets avez-vous d’ores et déjà réalisés ?</t>
@@ -1088,12 +1078,13 @@
   </sheetPr>
   <dimension ref="A1:N164"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="37.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="63.7"/>
@@ -1101,7 +1092,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="23.22"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1145,7 +1136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="247.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1179,6 +1170,9 @@
       <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D3" s="1" t="n">
+        <v>8</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1351,7 +1345,7 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
@@ -1544,7 +1538,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="1" t="s">
         <v>69</v>
       </c>
@@ -1758,11 +1752,14 @@
       <c r="C39" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D39" s="1" t="n">
+        <v>33</v>
+      </c>
       <c r="E39" s="1" t="s">
         <v>97</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>53</v>
@@ -1782,10 +1779,10 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -1794,10 +1791,10 @@
         <v>97</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>31</v>
@@ -1814,10 +1811,10 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -1826,10 +1823,10 @@
         <v>97</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>31</v>
@@ -1846,16 +1843,16 @@
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>97</v>
       </c>
       <c r="F45" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>18</v>
@@ -1872,10 +1869,10 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -1884,10 +1881,10 @@
         <v>97</v>
       </c>
       <c r="F47" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>31</v>
@@ -1904,16 +1901,16 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>97</v>
       </c>
       <c r="F49" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>46</v>
@@ -1922,13 +1919,13 @@
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="F50" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>99</v>
@@ -1941,17 +1938,17 @@
         <v>32</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>22</v>
@@ -1959,11 +1956,14 @@
       <c r="C52" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D52" s="1" t="n">
+        <v>24</v>
+      </c>
       <c r="E52" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>53</v>
@@ -1976,29 +1976,29 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F54" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>31</v>
@@ -2010,27 +2010,27 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F56" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>31</v>
@@ -2042,27 +2042,27 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E57" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F58" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>31</v>
@@ -2074,27 +2074,27 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F60" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>31</v>
@@ -2106,21 +2106,21 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E61" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="G62" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>18</v>
@@ -2132,27 +2132,27 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F64" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>31</v>
@@ -2164,71 +2164,71 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E65" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F66" s="1" t="s">
+      <c r="G66" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" customFormat="false" ht="673.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="695.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="F67" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F67" s="1" t="s">
+      <c r="G67" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>84</v>
       </c>
       <c r="I67" s="1"/>
       <c r="M67" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E68" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="E69" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="F69" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F69" s="1" t="s">
+      <c r="G69" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>84</v>
@@ -2237,27 +2237,27 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="E71" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="F71" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>84</v>
@@ -2266,27 +2266,27 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E72" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F73" s="1" t="s">
+      <c r="G73" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>84</v>
@@ -2295,7 +2295,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E74" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L74" s="1" t="s">
         <v>25</v>
@@ -2306,13 +2306,13 @@
         <v>22</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F75" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G75" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>84</v>
@@ -2321,27 +2321,27 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E76" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E77" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F77" s="2" t="s">
+      <c r="G77" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>18</v>
@@ -2350,41 +2350,41 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E78" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E79" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F79" s="1" t="s">
+      <c r="G79" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>31</v>
       </c>
       <c r="I79" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="L79" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="L79" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="F80" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>99</v>
@@ -2397,17 +2397,17 @@
         <v>19</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E81" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>22</v>
@@ -2415,11 +2415,14 @@
       <c r="C82" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D82" s="1" t="n">
+        <v>36</v>
+      </c>
       <c r="E82" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>53</v>
@@ -2434,27 +2437,27 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E83" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F84" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G84" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>31</v>
@@ -2466,21 +2469,21 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E85" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F86" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E86" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="G86" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>18</v>
@@ -2492,27 +2495,27 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E87" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F88" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G88" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>31</v>
@@ -2524,21 +2527,21 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E89" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F90" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E90" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F90" s="1" t="s">
+      <c r="G90" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>46</v>
@@ -2547,13 +2550,13 @@
     </row>
     <row r="91" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E91" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="F91" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>190</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>99</v>
@@ -2566,17 +2569,17 @@
         <v>19</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E92" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>22</v>
@@ -2584,11 +2587,14 @@
       <c r="C93" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D93" s="1" t="n">
+        <v>21</v>
+      </c>
       <c r="E93" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>53</v>
@@ -2603,27 +2609,27 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E94" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F95" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G95" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>31</v>
@@ -2635,27 +2641,27 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E96" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F97" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G97" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>31</v>
@@ -2667,21 +2673,21 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E98" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F99" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E99" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="G99" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>18</v>
@@ -2693,27 +2699,27 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E100" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F101" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G101" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>31</v>
@@ -2725,21 +2731,21 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E102" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F103" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E103" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F103" s="1" t="s">
+      <c r="G103" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>46</v>
@@ -2748,13 +2754,13 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E104" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E104" s="1" t="s">
+      <c r="F104" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>99</v>
@@ -2767,17 +2773,17 @@
         <v>19</v>
       </c>
       <c r="M104" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E105" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>22</v>
@@ -2785,11 +2791,14 @@
       <c r="C106" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D106" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E106" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F106" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>53</v>
@@ -2804,27 +2813,27 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E107" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F108" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G108" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>31</v>
@@ -2836,21 +2845,21 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E109" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F110" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F110" s="2" t="s">
+      <c r="G110" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>18</v>
@@ -2862,27 +2871,27 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E111" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F112" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G112" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="H112" s="1" t="s">
         <v>31</v>
@@ -2894,24 +2903,24 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E113" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F114" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E114" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F114" s="1" t="s">
+      <c r="G114" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="G114" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>46</v>
@@ -2920,13 +2929,13 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E115" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E115" s="1" t="s">
+      <c r="F115" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>99</v>
@@ -2939,17 +2948,17 @@
         <v>19</v>
       </c>
       <c r="M115" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E116" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>22</v>
@@ -2957,11 +2966,14 @@
       <c r="C117" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D117" s="1" t="n">
+        <v>27</v>
+      </c>
       <c r="E117" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F117" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="G117" s="1" t="s">
         <v>53</v>
@@ -2976,7 +2988,7 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E118" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J118" s="1" t="s">
         <v>32</v>
@@ -2984,22 +2996,22 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F119" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G119" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>31</v>
@@ -3008,27 +3020,27 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F121" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G121" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>31</v>
@@ -3040,21 +3052,21 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E122" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F123" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="E123" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="G123" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H123" s="1" t="s">
         <v>18</v>
@@ -3066,7 +3078,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E124" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J124" s="1" t="s">
         <v>32</v>
@@ -3074,22 +3086,22 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F125" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G125" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="G125" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="H125" s="1" t="s">
         <v>31</v>
@@ -3098,21 +3110,21 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E126" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F127" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E127" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F127" s="1" t="s">
+      <c r="G127" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>46</v>
@@ -3121,33 +3133,33 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E128" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E128" s="1" t="s">
+      <c r="F128" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="F128" s="1" t="s">
+      <c r="G128" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="G128" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="H128" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I128" s="1"/>
       <c r="M128" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E129" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>22</v>
@@ -3155,14 +3167,17 @@
       <c r="C130" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D130" s="1" t="n">
+        <v>15</v>
+      </c>
       <c r="E130" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F130" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="F130" s="1" t="s">
-        <v>249</v>
-      </c>
       <c r="G130" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H130" s="1" t="s">
         <v>18</v>
@@ -3171,27 +3186,27 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E131" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B132" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F132" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G132" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="G132" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="H132" s="1" t="s">
         <v>31</v>
@@ -3203,27 +3218,27 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E133" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F134" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G134" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="G134" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="H134" s="1" t="s">
         <v>31</v>
@@ -3233,23 +3248,23 @@
         <v>32</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E135" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F136" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="E136" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="F136" s="2" t="s">
-        <v>262</v>
-      </c>
       <c r="G136" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H136" s="1" t="s">
         <v>18</v>
@@ -3261,27 +3276,27 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E137" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F138" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G138" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="H138" s="1" t="s">
         <v>31</v>
@@ -3293,21 +3308,21 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E139" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F140" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="E140" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="F140" s="1" t="s">
+      <c r="G140" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="H140" s="1" t="s">
         <v>46</v>
@@ -3316,13 +3331,13 @@
     </row>
     <row r="141" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E141" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E141" s="1" t="s">
+      <c r="F141" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>99</v>
@@ -3335,17 +3350,17 @@
         <v>19</v>
       </c>
       <c r="M141" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E142" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>22</v>
@@ -3353,11 +3368,14 @@
       <c r="C143" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D143" s="1" t="n">
+        <v>12</v>
+      </c>
       <c r="E143" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F143" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="F143" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="G143" s="1" t="s">
         <v>53</v>
@@ -3369,27 +3387,27 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E144" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B145" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>275</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F145" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G145" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="H145" s="1" t="s">
         <v>31</v>
@@ -3401,21 +3419,21 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E146" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F147" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="E147" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F147" s="2" t="s">
-        <v>279</v>
-      </c>
       <c r="G147" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H147" s="1" t="s">
         <v>18</v>
@@ -3427,27 +3445,27 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E148" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F149" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G149" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="G149" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="H149" s="1" t="s">
         <v>31</v>
@@ -3459,36 +3477,36 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E150" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F151" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E151" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F151" s="1" t="s">
+      <c r="G151" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="G151" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="H151" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I151" s="1"/>
     </row>
-    <row r="152" customFormat="false" ht="281.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="292.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E152" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E152" s="1" t="s">
+      <c r="F152" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="F152" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>99</v>
@@ -3501,30 +3519,32 @@
         <v>19</v>
       </c>
       <c r="M152" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E153" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="D154" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="D154" s="2" t="n">
+        <v>18</v>
+      </c>
       <c r="E154" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F154" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="F154" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="G154" s="1" t="s">
         <v>53</v>
@@ -3539,27 +3559,27 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E155" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H156" s="1" t="s">
         <v>31</v>
@@ -3571,27 +3591,27 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E157" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H158" s="1" t="s">
         <v>31</v>
@@ -3603,21 +3623,21 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E159" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>18</v>
@@ -3629,27 +3649,27 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E161" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H162" s="1" t="s">
         <v>31</v>
@@ -3658,21 +3678,21 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E163" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="G164" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F164" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="G164" s="1" t="s">
-        <v>306</v>
       </c>
       <c r="H164" s="1" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
modifications du fichier de données
</commit_message>
<xml_diff>
--- a/data/questions_combinees.xlsx
+++ b/data/questions_combinees.xlsx
@@ -8,19 +8,19 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="304">
   <si>
     <t xml:space="preserve">Numero</t>
   </si>
@@ -49,13 +49,16 @@
     <t xml:space="preserve">Affichage</t>
   </si>
   <si>
-    <t xml:space="preserve">...8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">...7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Choix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observation</t>
   </si>
   <si>
     <t xml:space="preserve">TexteTheme</t>
@@ -83,6 +86,9 @@
     <t xml:space="preserve">Mono</t>
   </si>
   <si>
+    <t xml:space="preserve">Maturite</t>
+  </si>
+  <si>
     <t xml:space="preserve">Le changement climatique appelle à repenser l’aménagement en faveur d’espaces urbains vivables.
 Concrètement, il s’agit de combiner différentes expertises pour envisager des solutions globales : qualité du cadre de vie, revitalisation de quartier, développement des mobilités douces, Nature en ville, protection de la biodiversité, gestion des nuisances, gestion des déchets du BTP, etc. Cette approche s’applique aussi bien à l’échelle du quartier (écoquartiers) que de l’îlot (cour d’école résiliente). </t>
   </si>
@@ -99,9 +105,6 @@
     <t xml:space="preserve">Oui ;Non ;Je ne sais pas ;Non applicable à l’échelle de mon syndicat (SSI syndicat)</t>
   </si>
   <si>
-    <t xml:space="preserve">o</t>
-  </si>
-  <si>
     <t xml:space="preserve">8.2</t>
   </si>
   <si>
@@ -130,6 +133,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cadre de vie agréable et apaisé ;Espace public et interaction sociale ;Accessibilité et mobilités douces ;Végétalisation ;Lutte contre la surchauffe urbaine ;Protection de la biodiversité ;Bien-être et santé ;Economie circulaire des matériaux et gestion des déchets du BTP ;Association des parties prenantes ;Evaluation socio-économique des projets d’aménagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projet</t>
   </si>
   <si>
     <t xml:space="preserve">9</t>
@@ -143,6 +149,9 @@
     <t xml:space="preserve">Oui ;Non, pas à ce stade </t>
   </si>
   <si>
+    <t xml:space="preserve">Accompagnement</t>
+  </si>
+  <si>
     <t xml:space="preserve">10</t>
   </si>
   <si>
@@ -153,8 +162,7 @@
     <t xml:space="preserve">Bâtir un quartier durable et résilient ;Revitaliser en s’adaptant au changement climatique ;Développer et adapter son territoire de montagne au changement climatique ; Agir pour l’école de demain ;Développer des solutions contre la surchauffe urbaine;Mobiliser des solutions fondées sur la nature pour une ville apaisée ;Aménager en intégrant les enjeux environnementaux (santé, bruit, vibrations, qualité de l’air) ;Favoriser l’écoconstruction, gérer des déchets du BTP, valoriser les matériaux du BTP dans les projets de construction et d’aménagement ;Mettre en œuvre des démarche participatives</t>
   </si>
   <si>
-    <t xml:space="preserve">Multichoix
-2 MAX</t>
+    <t xml:space="preserve">Multichoix 2 MAX</t>
   </si>
   <si>
     <t xml:space="preserve">11</t>
@@ -167,6 +175,9 @@
   </si>
   <si>
     <t xml:space="preserve">textarea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas obligatoire</t>
   </si>
   <si>
     <t xml:space="preserve">5</t>
@@ -227,9 +238,6 @@
     <t xml:space="preserve">Monter en compétences sur les items de la transition et l’adaptation ;Renforcer projets et/ou documents de planification au regard des enjeux de transition écologique et de résilience ;Prioriser et mettre en cohérence stratégies et projets ;Renforcer le diagnostic de résilience / adaptation au changement climatique ;Fédérer les acteurs, mettre en place une gouvernance élargie ;Evaluer la démarche au regard des enjeux de transition et résilience ;Elaborer une démarche globale (acculturation, portrait de territoire, stratégie et mise en récits, plan d’actions et évaluation)</t>
   </si>
   <si>
-    <t xml:space="preserve">Multichoix 2 MAX</t>
-  </si>
-  <si>
     <t xml:space="preserve">7</t>
   </si>
   <si>
@@ -252,12 +260,12 @@
     <t xml:space="preserve">Dynamique de transition territoriale;Aménagement urbain durable;Territoire intelligent;Sobriété foncière;Transition énergétique;Mobilités décarbonées;Infrastructures résilientes (réseaux routiers, ouvrages d’art, bâtiments, infrastructures portuaires);Gestion et prévention des risques naturels;Nature en ville;Gestion intégrée de l’eau;Gestion du Gestion du littoral</t>
   </si>
   <si>
+    <t xml:space="preserve">Multichoix 3 MAX</t>
+  </si>
+  <si>
     <t xml:space="preserve">Si Gestion du littoral</t>
   </si>
   <si>
-    <t xml:space="preserve">Multi ( Max 3)</t>
-  </si>
-  <si>
     <t xml:space="preserve">40</t>
   </si>
   <si>
@@ -276,9 +284,6 @@
     <t xml:space="preserve">Obligatoire</t>
   </si>
   <si>
-    <t xml:space="preserve">Texte</t>
-  </si>
-  <si>
     <t xml:space="preserve">51</t>
   </si>
   <si>
@@ -291,9 +296,6 @@
     <t xml:space="preserve">select</t>
   </si>
   <si>
-    <t xml:space="preserve">Mr Mme</t>
-  </si>
-  <si>
     <t xml:space="preserve">52</t>
   </si>
   <si>
@@ -319,9 +321,6 @@
   </si>
   <si>
     <t xml:space="preserve">Téléphone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Text</t>
   </si>
   <si>
     <t xml:space="preserve">33</t>
@@ -547,9 +546,6 @@
   </si>
   <si>
     <t xml:space="preserve">inline-block</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pas obligatoire</t>
   </si>
   <si>
     <t xml:space="preserve">36</t>
@@ -980,12 +976,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1001,6 +997,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -1046,17 +1048,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1071,28 +1081,137 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N164"/>
+  <dimension ref="A1:O164"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A68" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G75" activeCellId="0" sqref="G75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M78" activeCellId="0" sqref="M78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="37.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="63.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="46.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="23.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="75.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="12.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="23.22"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1135,583 +1254,629 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="247.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="104.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M15" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="70.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I27" s="1"/>
-      <c r="J27" s="1" t="s">
+      <c r="J27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E28" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I31" s="1"/>
-      <c r="J31" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I33" s="1"/>
-      <c r="J33" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="I34" s="1"/>
-      <c r="J34" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I35" s="1"/>
-      <c r="J35" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I36" s="1"/>
-      <c r="K36" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
@@ -1727,30 +1892,33 @@
         <v>99</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N37" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D39" s="1" t="n">
         <v>33</v>
@@ -1762,22 +1930,25 @@
         <v>98</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E40" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>102</v>
       </c>
@@ -1785,7 +1956,7 @@
         <v>103</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>97</v>
@@ -1797,19 +1968,22 @@
         <v>105</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I41" s="1"/>
       <c r="J41" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K41" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E42" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>106</v>
       </c>
@@ -1817,7 +1991,7 @@
         <v>103</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>97</v>
@@ -1829,14 +2003,17 @@
         <v>108</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="1" t="s">
         <v>97</v>
       </c>
@@ -1855,19 +2032,22 @@
         <v>111</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K45" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E46" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>112</v>
       </c>
@@ -1875,7 +2055,7 @@
         <v>109</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>97</v>
@@ -1887,19 +2067,22 @@
         <v>114</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I47" s="1"/>
       <c r="J47" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="K47" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>115</v>
       </c>
@@ -1913,7 +2096,7 @@
         <v>117</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I49" s="1"/>
     </row>
@@ -1931,17 +2114,20 @@
         <v>99</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I50" s="1"/>
       <c r="J50" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K50" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N50" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="1" t="s">
         <v>119</v>
       </c>
@@ -1951,10 +2137,10 @@
         <v>122</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D52" s="1" t="n">
         <v>24</v>
@@ -1966,17 +2152,20 @@
         <v>120</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I52" s="1"/>
       <c r="J52" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K52" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
         <v>119</v>
       </c>
@@ -1989,7 +2178,7 @@
         <v>124</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>119</v>
@@ -2001,19 +2190,22 @@
         <v>126</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I54" s="1"/>
       <c r="J54" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K54" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>127</v>
       </c>
@@ -2021,7 +2213,7 @@
         <v>124</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>119</v>
@@ -2033,19 +2225,22 @@
         <v>129</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K56" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E57" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>130</v>
       </c>
@@ -2053,7 +2248,7 @@
         <v>124</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>119</v>
@@ -2065,19 +2260,22 @@
         <v>132</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I58" s="1"/>
       <c r="J58" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K58" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>133</v>
       </c>
@@ -2085,7 +2283,7 @@
         <v>124</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>119</v>
@@ -2097,19 +2295,22 @@
         <v>135</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I60" s="1"/>
       <c r="J60" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K60" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E61" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>136</v>
       </c>
@@ -2123,19 +2324,22 @@
         <v>111</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K62" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>138</v>
       </c>
@@ -2143,7 +2347,7 @@
         <v>136</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>119</v>
@@ -2155,19 +2359,22 @@
         <v>140</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="K64" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E65" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>141</v>
       </c>
@@ -2181,11 +2388,11 @@
         <v>143</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" customFormat="false" ht="695.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="69" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>144</v>
       </c>
@@ -2199,19 +2406,25 @@
         <v>147</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I67" s="1"/>
-      <c r="M67" s="2" t="s">
+      <c r="J67" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M67" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="N67" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E68" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>149</v>
       </c>
@@ -2231,16 +2444,22 @@
         <v>152</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I69" s="1"/>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J69" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M69" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>153</v>
       </c>
@@ -2260,16 +2479,22 @@
         <v>155</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I71" s="1"/>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J71" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M71" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E72" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>156</v>
       </c>
@@ -2289,21 +2514,25 @@
         <v>158</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I73" s="1"/>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J73" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M73" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E74" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="L74" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M74" s="1"/>
+    </row>
+    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>145</v>
@@ -2315,11 +2544,17 @@
         <v>160</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I75" s="1"/>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J75" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M75" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E76" s="1" t="s">
         <v>145</v>
       </c>
@@ -2329,7 +2564,7 @@
         <v>161</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>162</v>
@@ -2344,16 +2579,22 @@
         <v>164</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I77" s="1"/>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J77" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M77" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E78" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>165</v>
       </c>
@@ -2367,1335 +2608,1463 @@
         <v>167</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="L79" s="1" t="s">
-        <v>169</v>
+      <c r="M79" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="F80" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>99</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I80" s="1"/>
       <c r="J80" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M80" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K80" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N80" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E81" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E81" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="B82" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D82" s="1" t="n">
         <v>36</v>
       </c>
       <c r="E82" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F82" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="G82" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I82" s="1"/>
       <c r="J82" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K82" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E83" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F84" s="1" t="s">
+      <c r="G84" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G84" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="H84" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I84" s="1"/>
       <c r="J84" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K84" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E85" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F86" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>111</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I86" s="1"/>
       <c r="J86" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K86" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E87" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F88" s="1" t="s">
+      <c r="G88" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G88" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="H88" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I88" s="1"/>
       <c r="J88" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="K88" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E89" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F90" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E90" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F90" s="1" t="s">
+      <c r="G90" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="G90" s="1" t="s">
+      <c r="H90" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I90" s="1"/>
+    </row>
+    <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H90" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I90" s="1"/>
-    </row>
-    <row r="91" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="s">
+      <c r="E91" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="F91" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>99</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I91" s="1"/>
       <c r="J91" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M91" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K91" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N91" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E92" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E92" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="B93" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D93" s="1" t="n">
         <v>21</v>
       </c>
       <c r="E93" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F93" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="G93" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I93" s="1"/>
       <c r="J93" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K93" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E94" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="C95" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F95" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F95" s="2" t="s">
+      <c r="G95" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G95" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="H95" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I95" s="1"/>
       <c r="J95" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K95" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E96" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H97" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E96" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="H97" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="I97" s="1"/>
       <c r="J97" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K97" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E98" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F99" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>200</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>111</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I99" s="1"/>
       <c r="J99" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K99" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E100" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F101" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F101" s="1" t="s">
+      <c r="G101" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="G101" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="H101" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I101" s="1"/>
       <c r="J101" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="K101" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E102" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F103" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E103" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F103" s="1" t="s">
+      <c r="G103" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="G103" s="1" t="s">
+      <c r="H103" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I103" s="1"/>
+    </row>
+    <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="H103" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I103" s="1"/>
-    </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="1" t="s">
+      <c r="E104" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E104" s="1" t="s">
+      <c r="F104" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>99</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I104" s="1"/>
       <c r="J104" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M104" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K104" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N104" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E105" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E105" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="B106" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D106" s="1" t="n">
         <v>30</v>
       </c>
       <c r="E106" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F106" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="F106" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="G106" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I106" s="1"/>
       <c r="J106" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K106" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E107" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="C108" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F108" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F108" s="1" t="s">
+      <c r="G108" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="G108" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="H108" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I108" s="1"/>
       <c r="J108" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K108" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E109" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F110" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F110" s="2" t="s">
+      <c r="G110" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="G110" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="H110" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I110" s="1"/>
       <c r="J110" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K110" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E111" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F112" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F112" s="1" t="s">
+      <c r="G112" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G112" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="H112" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I112" s="1"/>
       <c r="J112" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="K112" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E113" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J113" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="s">
+      <c r="E114" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F114" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E114" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F114" s="1" t="s">
+      <c r="G114" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G114" s="1" t="s">
+      <c r="H114" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I114" s="1"/>
+    </row>
+    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="H114" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I114" s="1"/>
-    </row>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="1" t="s">
+      <c r="E115" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E115" s="1" t="s">
+      <c r="F115" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>99</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I115" s="1"/>
       <c r="J115" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M115" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K115" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N115" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E116" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E116" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="B117" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D117" s="1" t="n">
         <v>27</v>
       </c>
       <c r="E117" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F117" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="F117" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="G117" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I117" s="1"/>
       <c r="J117" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K117" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E118" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J118" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J118" s="1"/>
+    </row>
+    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H119" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="1" t="s">
+      <c r="I119" s="1"/>
+      <c r="J119" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="K119" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E120" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H119" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I119" s="1"/>
-    </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E120" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="1" t="s">
+      <c r="C121" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F121" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F121" s="1" t="s">
+      <c r="G121" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G121" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="H121" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I121" s="1"/>
       <c r="J121" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K121" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E122" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F123" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>239</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>111</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I123" s="1"/>
       <c r="J123" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K123" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E124" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J124" s="1"/>
+    </row>
+    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I125" s="1"/>
+      <c r="J125" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="K125" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E126" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I127" s="1"/>
+    </row>
+    <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="H128" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E124" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J124" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G125" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="H125" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I125" s="1"/>
-    </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E126" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="H127" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I127" s="1"/>
-    </row>
-    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="1" t="s">
+      <c r="I128" s="1"/>
+      <c r="J128" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K128" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N128" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E129" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E128" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="G128" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="H128" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I128" s="1"/>
-      <c r="M128" s="1" t="s">
+    </row>
+    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E129" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="1" t="s">
-        <v>251</v>
-      </c>
       <c r="B130" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D130" s="1" t="n">
         <v>15</v>
       </c>
       <c r="E130" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F130" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="F130" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="G130" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I130" s="1"/>
+      <c r="J130" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K130" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E131" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="H130" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I130" s="1"/>
-    </row>
-    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E131" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="1" t="s">
+      <c r="B132" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="C132" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F132" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C132" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F132" s="1" t="s">
+      <c r="G132" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G132" s="1" t="s">
-        <v>256</v>
-      </c>
       <c r="H132" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I132" s="1"/>
       <c r="J132" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K132" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E133" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F134" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F134" s="2" t="s">
+      <c r="G134" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="G134" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="H134" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I134" s="1"/>
       <c r="J134" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K134" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E135" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F136" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F136" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="G136" s="1" t="s">
         <v>111</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I136" s="1"/>
       <c r="J136" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K136" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E137" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F138" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F138" s="1" t="s">
+      <c r="G138" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="G138" s="1" t="s">
-        <v>264</v>
-      </c>
       <c r="H138" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I138" s="1"/>
       <c r="J138" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="K138" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E139" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F140" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="E140" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F140" s="1" t="s">
+      <c r="G140" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="G140" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="H140" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I140" s="1"/>
     </row>
     <row r="141" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E141" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="E141" s="1" t="s">
+      <c r="F141" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>99</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I141" s="1"/>
       <c r="J141" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M141" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K141" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N141" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E142" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D143" s="1" t="n">
         <v>12</v>
       </c>
       <c r="E143" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F143" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F143" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="G143" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H143" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I143" s="1"/>
-    </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K143" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E144" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B145" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="C145" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F145" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C145" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="F145" s="1" t="s">
+      <c r="G145" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="G145" s="1" t="s">
-        <v>276</v>
-      </c>
       <c r="H145" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I145" s="1"/>
       <c r="J145" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K145" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E146" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F147" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="F147" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>111</v>
       </c>
       <c r="H147" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I147" s="1"/>
       <c r="J147" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K147" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E148" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F149" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="F149" s="1" t="s">
+      <c r="G149" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="G149" s="1" t="s">
-        <v>281</v>
-      </c>
       <c r="H149" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I149" s="1"/>
       <c r="J149" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="K149" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E150" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F151" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E151" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="F151" s="1" t="s">
+      <c r="G151" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="G151" s="1" t="s">
-        <v>284</v>
-      </c>
       <c r="H151" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I151" s="1"/>
     </row>
     <row r="152" customFormat="false" ht="292.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E152" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E152" s="1" t="s">
+      <c r="F152" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="F152" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>99</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I152" s="1"/>
       <c r="J152" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M152" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K152" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N152" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E153" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="1" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E153" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="1" t="s">
-        <v>289</v>
-      </c>
       <c r="B154" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D154" s="2" t="n">
         <v>18</v>
       </c>
       <c r="E154" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F154" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F154" s="1" t="s">
-        <v>287</v>
-      </c>
       <c r="G154" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I154" s="1"/>
       <c r="J154" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K154" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E155" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B156" s="1" t="s">
+      <c r="C156" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F156" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="C156" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F156" s="1" t="s">
+      <c r="G156" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="G156" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="H156" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I156" s="1"/>
       <c r="J156" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K156" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E157" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H158" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E157" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F158" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="G158" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="H158" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="I158" s="1"/>
       <c r="J158" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="K158" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E159" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F160" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F160" s="2" t="s">
-        <v>298</v>
       </c>
       <c r="G160" s="1" t="s">
         <v>111</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I160" s="1"/>
       <c r="J160" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="K160" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E161" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F162" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="B162" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F162" s="1" t="s">
+      <c r="G162" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="G162" s="1" t="s">
+      <c r="H162" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I162" s="1"/>
+      <c r="J162" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="K162" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E163" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="H162" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I162" s="1"/>
-    </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E163" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="1" t="s">
+      <c r="E164" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F164" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="E164" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F164" s="1" t="s">
+      <c r="G164" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="G164" s="1" t="s">
-        <v>304</v>
-      </c>
       <c r="H164" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I164" s="1"/>
     </row>

</xml_diff>

<commit_message>
Mise en place nbre max de réponses
</commit_message>
<xml_diff>
--- a/data/questions_combinees.xlsx
+++ b/data/questions_combinees.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="305">
   <si>
     <t xml:space="preserve">Numero</t>
   </si>
@@ -712,9 +712,6 @@
   </si>
   <si>
     <t xml:space="preserve">Renforcer la place de l’arbre dans la ville;Mettre en œuvre d’autres Solutions Fondées sur la Nature (SFN;Préserver la qualité des sols</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">32</t>
@@ -1084,8 +1081,8 @@
   </sheetPr>
   <dimension ref="A1:O164"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M77" activeCellId="0" sqref="M77"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J113" activeCellId="0" sqref="J113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3061,22 +3058,19 @@
       <c r="E113" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="J113" s="1" t="s">
-        <v>223</v>
-      </c>
     </row>
     <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>209</v>
       </c>
       <c r="F114" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G114" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="G114" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>49</v>
@@ -3085,13 +3079,13 @@
     </row>
     <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E115" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E115" s="1" t="s">
+      <c r="F115" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>99</v>
@@ -3107,17 +3101,17 @@
         <v>21</v>
       </c>
       <c r="N115" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E116" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>24</v>
@@ -3129,10 +3123,10 @@
         <v>27</v>
       </c>
       <c r="E117" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F117" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="G117" s="1" t="s">
         <v>57</v>
@@ -3150,27 +3144,27 @@
     </row>
     <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E118" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F119" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G119" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>32</v>
@@ -3185,27 +3179,27 @@
     </row>
     <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F121" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G121" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>32</v>
@@ -3220,18 +3214,18 @@
     </row>
     <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E122" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F123" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>111</v>
@@ -3249,27 +3243,27 @@
     </row>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E124" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F125" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G125" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="G125" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="H125" s="1" t="s">
         <v>32</v>
@@ -3284,21 +3278,21 @@
     </row>
     <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E126" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F127" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E127" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F127" s="1" t="s">
+      <c r="G127" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>49</v>
@@ -3307,16 +3301,16 @@
     </row>
     <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E128" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E128" s="1" t="s">
+      <c r="F128" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="F128" s="1" t="s">
+      <c r="G128" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="G128" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="H128" s="1" t="s">
         <v>19</v>
@@ -3329,17 +3323,17 @@
         <v>21</v>
       </c>
       <c r="N128" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E129" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>24</v>
@@ -3351,13 +3345,13 @@
         <v>15</v>
       </c>
       <c r="E130" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F130" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="F130" s="1" t="s">
-        <v>249</v>
-      </c>
       <c r="G130" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H130" s="1" t="s">
         <v>19</v>
@@ -3372,27 +3366,27 @@
     </row>
     <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E131" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B132" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F132" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G132" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="G132" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="H132" s="1" t="s">
         <v>32</v>
@@ -3407,27 +3401,27 @@
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E133" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F134" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G134" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="G134" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="H134" s="1" t="s">
         <v>32</v>
@@ -3442,18 +3436,18 @@
     </row>
     <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E135" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F136" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="F136" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="G136" s="1" t="s">
         <v>111</v>
@@ -3471,27 +3465,27 @@
     </row>
     <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E137" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F138" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G138" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="H138" s="1" t="s">
         <v>32</v>
@@ -3506,21 +3500,21 @@
     </row>
     <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E139" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F140" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="E140" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="F140" s="1" t="s">
+      <c r="G140" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="H140" s="1" t="s">
         <v>49</v>
@@ -3529,13 +3523,13 @@
     </row>
     <row r="141" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E141" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E141" s="1" t="s">
+      <c r="F141" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>99</v>
@@ -3551,17 +3545,17 @@
         <v>21</v>
       </c>
       <c r="N141" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E142" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>24</v>
@@ -3573,10 +3567,10 @@
         <v>12</v>
       </c>
       <c r="E143" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F143" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="F143" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="G143" s="1" t="s">
         <v>57</v>
@@ -3591,27 +3585,27 @@
     </row>
     <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E144" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B145" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>275</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F145" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G145" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="H145" s="1" t="s">
         <v>32</v>
@@ -3626,18 +3620,18 @@
     </row>
     <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E146" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F147" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F147" s="2" t="s">
-        <v>279</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>111</v>
@@ -3655,27 +3649,27 @@
     </row>
     <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E148" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F149" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G149" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="G149" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="H149" s="1" t="s">
         <v>32</v>
@@ -3690,21 +3684,21 @@
     </row>
     <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E150" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F151" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E151" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F151" s="1" t="s">
+      <c r="G151" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="G151" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="H151" s="1" t="s">
         <v>49</v>
@@ -3713,13 +3707,13 @@
     </row>
     <row r="152" customFormat="false" ht="292.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E152" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E152" s="1" t="s">
+      <c r="F152" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="F152" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>99</v>
@@ -3735,17 +3729,17 @@
         <v>21</v>
       </c>
       <c r="N152" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E153" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>24</v>
@@ -3757,10 +3751,10 @@
         <v>18</v>
       </c>
       <c r="E154" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F154" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="F154" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="G154" s="1" t="s">
         <v>57</v>
@@ -3778,27 +3772,27 @@
     </row>
     <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E155" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>292</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F156" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="G156" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="G156" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="H156" s="1" t="s">
         <v>32</v>
@@ -3813,27 +3807,27 @@
     </row>
     <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E157" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F158" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="G158" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="G158" s="1" t="s">
-        <v>297</v>
       </c>
       <c r="H158" s="1" t="s">
         <v>32</v>
@@ -3848,18 +3842,18 @@
     </row>
     <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E159" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F160" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F160" s="2" t="s">
-        <v>299</v>
       </c>
       <c r="G160" s="1" t="s">
         <v>111</v>
@@ -3877,27 +3871,27 @@
     </row>
     <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E161" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F162" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G162" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="G162" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="H162" s="1" t="s">
         <v>32</v>
@@ -3912,21 +3906,21 @@
     </row>
     <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E163" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F164" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="E164" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F164" s="1" t="s">
+      <c r="G164" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="G164" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="H164" s="1" t="s">
         <v>49</v>

</xml_diff>